<commit_message>
adding the second plate data from 1/14/20
</commit_message>
<xml_diff>
--- a/maps/1_14_19_rat_plate1.xlsx
+++ b/maps/1_14_19_rat_plate1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iotabio-my.sharepoint.com/personal/ryan_iota_bio/Documents/code/multiplex/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{683C6896-6F78-45DF-A228-4E7CDCC331D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C4D39476-C902-4E9D-A60B-E101A653F08E}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{683C6896-6F78-45DF-A228-4E7CDCC331D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4650888D-8D0E-42E2-A1F8-21CD30521DDB}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="-4770" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27240" yWindow="-3990" windowWidth="24510" windowHeight="14175" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>splanchnic stim</t>
   </si>
   <si>
-    <t>1_14_19_rat_plate1</t>
-  </si>
-  <si>
     <t>X1, X2, X3</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>X36,X37,X38,X39</t>
+  </si>
+  <si>
+    <t>C:\Users\Ryan\OneDrive - Iota Bio\data\multiplex\1_14_20_rat_plate1.xlsx</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -508,13 +508,13 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -525,13 +525,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -542,13 +542,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -559,13 +559,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -576,13 +576,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -593,13 +593,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -610,13 +610,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -627,13 +627,13 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -644,13 +644,13 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -661,13 +661,13 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>